<commit_message>
Added .csv and .xlsx files
</commit_message>
<xml_diff>
--- a/labyrinth0.xlsx
+++ b/labyrinth0.xlsx
@@ -21,15 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="3">
   <si>
     <t>X</t>
   </si>
   <si>
     <t xml:space="preserve">M </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>G</t>
@@ -39,10 +36,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -64,13 +75,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,7 +426,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -459,15 +482,6 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
@@ -557,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -582,9 +596,6 @@
       <c r="G5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
       <c r="I5" t="s">
         <v>0</v>
       </c>
@@ -609,6 +620,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>